<commit_message>
Fixing special characters (ß to ss)
</commit_message>
<xml_diff>
--- a/doc/micro_api_parameter.xlsx
+++ b/doc/micro_api_parameter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24816"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14960" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mikro-API-Parameter" sheetId="5" r:id="rId1"/>
@@ -269,15 +269,9 @@
     <t>autobahn</t>
   </si>
   <si>
-    <t>außenbereich</t>
-  </si>
-  <si>
     <t>angespannt</t>
   </si>
   <si>
-    <t>anliegerstraße</t>
-  </si>
-  <si>
     <t>ausbildungsstaette</t>
   </si>
   <si>
@@ -293,9 +287,6 @@
     <t>bach</t>
   </si>
   <si>
-    <t>bundesstraße</t>
-  </si>
-  <si>
     <t>bahntrasse</t>
   </si>
   <si>
@@ -311,9 +302,6 @@
     <t>buerogebaeude</t>
   </si>
   <si>
-    <t>durchgangsstraße</t>
-  </si>
-  <si>
     <t>dorfgebiet</t>
   </si>
   <si>
@@ -392,9 +380,6 @@
     <t>hauptverkehrsader</t>
   </si>
   <si>
-    <t>hauptstraße</t>
-  </si>
-  <si>
     <t>hafen</t>
   </si>
   <si>
@@ -527,9 +512,6 @@
     <t>see</t>
   </si>
   <si>
-    <t>spielstraße</t>
-  </si>
-  <si>
     <t>s-bahnhof</t>
   </si>
   <si>
@@ -656,9 +638,6 @@
     <t>wohn_und_geschaeftshaeuser</t>
   </si>
   <si>
-    <t>fußgaengerzone</t>
-  </si>
-  <si>
     <t>einfamilienhaeuser</t>
   </si>
   <si>
@@ -795,6 +774,27 @@
   </si>
   <si>
     <t>Micro-Apiparameter</t>
+  </si>
+  <si>
+    <t>aussenbereich</t>
+  </si>
+  <si>
+    <t>begruendung_strasse</t>
+  </si>
+  <si>
+    <t>bundesstrasse</t>
+  </si>
+  <si>
+    <t>spielstrasse</t>
+  </si>
+  <si>
+    <t>hauptstrasse</t>
+  </si>
+  <si>
+    <t>anliegerstrasse</t>
+  </si>
+  <si>
+    <t>durchgangsstrasse</t>
   </si>
 </sst>
 </file>
@@ -1000,8 +1000,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="109">
+  <cellStyleXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1201,7 +1205,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="109">
+  <cellStyles count="113">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1256,6 +1260,8 @@
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1310,6 +1316,8 @@
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1580,7 +1588,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1590,7 +1598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
@@ -1604,7 +1612,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18">
       <c r="A1" s="17" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18">
@@ -1612,7 +1620,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="33" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>55</v>
@@ -1621,13 +1629,13 @@
         <v>8</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="33" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>6</v>
@@ -1636,13 +1644,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="33" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>7</v>
@@ -1651,13 +1659,13 @@
         <v>9</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="E5" s="29"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="30" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>10</v>
@@ -1670,7 +1678,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
@@ -1683,7 +1691,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>13</v>
@@ -1696,7 +1704,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>14</v>
@@ -1709,7 +1717,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>15</v>
@@ -1722,7 +1730,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>16</v>
@@ -1735,7 +1743,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>17</v>
@@ -1748,7 +1756,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>18</v>
@@ -1761,7 +1769,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>19</v>
@@ -1774,7 +1782,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>20</v>
@@ -1787,7 +1795,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>56</v>
@@ -1800,7 +1808,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>57</v>
@@ -1813,7 +1821,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>26</v>
@@ -1826,7 +1834,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>27</v>
@@ -1839,7 +1847,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>28</v>
@@ -1852,7 +1860,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>30</v>
@@ -1865,7 +1873,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>32</v>
@@ -1878,10 +1886,10 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>8</v>
@@ -1891,7 +1899,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>58</v>
@@ -1904,7 +1912,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>29</v>
@@ -1913,15 +1921,15 @@
         <v>8</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>31</v>
@@ -1930,13 +1938,13 @@
         <v>8</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E26" s="29"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>33</v>
@@ -1945,13 +1953,13 @@
         <v>8</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E27" s="29"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>34</v>
@@ -1960,28 +1968,28 @@
         <v>8</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E28" s="29"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E29" s="29"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>59</v>
@@ -1990,13 +1998,13 @@
         <v>8</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>60</v>
@@ -2009,7 +2017,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>35</v>
@@ -2022,7 +2030,7 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>36</v>
@@ -2035,7 +2043,7 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>37</v>
@@ -2048,7 +2056,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>62</v>
@@ -2061,7 +2069,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>61</v>
@@ -2074,7 +2082,7 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>38</v>
@@ -2087,7 +2095,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>39</v>
@@ -2100,7 +2108,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>40</v>
@@ -2113,7 +2121,7 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>41</v>
@@ -2122,15 +2130,15 @@
         <v>8</v>
       </c>
       <c r="D40" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="E40" s="29" t="s">
         <v>235</v>
-      </c>
-      <c r="E40" s="29" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>42</v>
@@ -2139,13 +2147,13 @@
         <v>11</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E41" s="29"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>43</v>
@@ -2154,13 +2162,13 @@
         <v>11</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E42" s="29"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>44</v>
@@ -2169,13 +2177,13 @@
         <v>11</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E43" s="29"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>45</v>
@@ -2184,13 +2192,13 @@
         <v>8</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E44" s="29"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>46</v>
@@ -2199,13 +2207,13 @@
         <v>11</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E45" s="29"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>47</v>
@@ -2214,13 +2222,13 @@
         <v>11</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E46" s="29"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>48</v>
@@ -2229,13 +2237,13 @@
         <v>11</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E47" s="29"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>49</v>
@@ -2244,13 +2252,13 @@
         <v>8</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E48" s="29"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>50</v>
@@ -2259,13 +2267,13 @@
         <v>11</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E49" s="29"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>51</v>
@@ -2274,13 +2282,13 @@
         <v>11</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E50" s="29"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>52</v>
@@ -2289,13 +2297,13 @@
         <v>11</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E51" s="29"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B52" s="13" t="s">
         <v>53</v>
@@ -2308,22 +2316,22 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C53" s="14" t="s">
         <v>11</v>
       </c>
       <c r="D53" s="35" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E53" s="29"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B54" s="13" t="s">
         <v>54</v>
@@ -2336,25 +2344,25 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C55" s="14" t="s">
         <v>11</v>
       </c>
       <c r="D55" s="35" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E55" s="29"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>8</v>
@@ -2364,10 +2372,10 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>8</v>
@@ -2377,7 +2385,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>63</v>
@@ -2390,7 +2398,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>64</v>
@@ -2403,10 +2411,10 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="26" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B60" s="27" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>8</v>
@@ -2429,8 +2437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE87"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="T5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2467,7 +2475,7 @@
   <sheetData>
     <row r="1" spans="1:31" ht="18">
       <c r="A1" s="17" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" thickBot="1"/>
@@ -2506,7 +2514,7 @@
         <v>32</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="M3" s="21" t="s">
         <v>29</v>
@@ -2521,7 +2529,7 @@
         <v>34</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="R3" s="15" t="s">
         <v>35</v>
@@ -2530,7 +2538,7 @@
         <v>36</v>
       </c>
       <c r="T3" s="15" t="s">
-        <v>37</v>
+        <v>240</v>
       </c>
       <c r="U3" s="15" t="s">
         <v>62</v>
@@ -2551,10 +2559,10 @@
         <v>54</v>
       </c>
       <c r="AA3" s="20" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="AB3" s="20" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="AC3" s="34" t="s">
         <v>63</v>
@@ -2563,7 +2571,7 @@
         <v>64</v>
       </c>
       <c r="AE3" s="22" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="15" thickTop="1">
@@ -2571,7 +2579,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>0</v>
@@ -2580,7 +2588,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>0</v>
@@ -2589,7 +2597,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>0</v>
@@ -2604,7 +2612,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>0</v>
@@ -2631,13 +2639,13 @@
         <v>0</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="W4" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="X4" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="Y4" s="5" t="s">
         <v>0</v>
@@ -2649,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="AB4" s="19" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AC4" s="5" t="s">
         <v>0</v>
@@ -2666,7 +2674,7 @@
         <v>65</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>0</v>
@@ -2675,7 +2683,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>22</v>
@@ -2684,64 +2692,64 @@
         <v>69</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>199</v>
+        <v>12</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="V5" s="9" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="W5" s="9" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="X5" s="9" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="Y5" s="9" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="Z5" s="9" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="AA5" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AB5" s="9" t="s">
         <v>23</v>
@@ -2753,7 +2761,7 @@
         <v>1</v>
       </c>
       <c r="AE5" s="9" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:31">
@@ -2761,73 +2769,73 @@
         <v>66</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>70</v>
+        <v>239</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>69</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>78</v>
+        <v>241</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="T6" s="9" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="U6" s="9" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="V6" s="9" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="W6" s="9" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="X6" s="9" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="Y6" s="9" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="Z6" s="9" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="AA6" s="9" t="s">
         <v>23</v>
@@ -2842,7 +2850,7 @@
         <v>2</v>
       </c>
       <c r="AE6" s="9" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:31">
@@ -2850,58 +2858,58 @@
         <v>67</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>78</v>
+        <v>241</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S7" s="9" t="s">
         <v>14</v>
       </c>
       <c r="T7" s="9" t="s">
-        <v>156</v>
+        <v>242</v>
       </c>
       <c r="V7" s="9" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="W7" s="9" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="X7" s="9" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="Z7" s="9" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="AA7" s="9" t="s">
         <v>2</v>
@@ -2923,57 +2931,57 @@
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="9" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="9" t="s">
-        <v>111</v>
+        <v>243</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="M8" s="23" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="R8" s="1"/>
       <c r="S8" s="9" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="T8" s="9" t="s">
-        <v>72</v>
+        <v>244</v>
       </c>
       <c r="V8" s="9" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="W8" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="X8" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="Z8" s="9" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="AA8" s="9" t="s">
         <v>1</v>
       </c>
       <c r="AB8" s="9" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="AC8" s="9" t="s">
         <v>4</v>
@@ -2985,50 +2993,50 @@
     </row>
     <row r="9" spans="1:31">
       <c r="A9" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="9" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>111</v>
+        <v>243</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="9" t="s">
-        <v>84</v>
+        <v>245</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="9" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="T9" s="9" t="s">
-        <v>84</v>
+        <v>245</v>
       </c>
       <c r="V9" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="W9" s="9" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="X9" s="9" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="Z9" s="1"/>
       <c r="AA9" s="9" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="AC9" s="9" t="s">
         <v>5</v>
@@ -3040,43 +3048,43 @@
     </row>
     <row r="10" spans="1:31">
       <c r="A10" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>84</v>
+        <v>245</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="9" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="9" t="s">
-        <v>111</v>
+        <v>243</v>
       </c>
       <c r="V10" s="9" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="W10" s="9" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="X10" s="9" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="Z10" s="1"/>
       <c r="AC10" s="1"/>
@@ -3084,43 +3092,43 @@
     </row>
     <row r="11" spans="1:31">
       <c r="A11" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="9" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="V11" s="9" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="W11" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="X11" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="Z11" s="1"/>
       <c r="AB11" s="1"/>
@@ -3129,18 +3137,18 @@
     </row>
     <row r="12" spans="1:31">
       <c r="A12" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="9" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="9" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -3156,13 +3164,13 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="W12" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="X12" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
@@ -3172,18 +3180,18 @@
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="9" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="9" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -3199,7 +3207,7 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
@@ -3212,18 +3220,18 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="9" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -3250,18 +3258,18 @@
     </row>
     <row r="15" spans="1:31">
       <c r="A15" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -3288,18 +3296,18 @@
     </row>
     <row r="16" spans="1:31">
       <c r="A16" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="9" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -3326,18 +3334,18 @@
     </row>
     <row r="17" spans="1:30">
       <c r="A17" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="9" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="9" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -3364,15 +3372,15 @@
     </row>
     <row r="18" spans="1:30">
       <c r="A18" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B18" s="1"/>
       <c r="D18" s="9" t="s">
-        <v>199</v>
+        <v>12</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="9" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -3399,15 +3407,15 @@
     </row>
     <row r="19" spans="1:30">
       <c r="A19" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B19" s="1"/>
       <c r="D19" s="9" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="9" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -3434,15 +3442,15 @@
     </row>
     <row r="20" spans="1:30">
       <c r="A20" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B20" s="1"/>
       <c r="D20" s="9" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="9" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -3469,15 +3477,15 @@
     </row>
     <row r="21" spans="1:30">
       <c r="A21" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B21" s="1"/>
       <c r="D21" s="9" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -3504,15 +3512,15 @@
     </row>
     <row r="22" spans="1:30">
       <c r="A22" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B22" s="1"/>
       <c r="D22" s="9" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="9" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -3539,11 +3547,11 @@
     </row>
     <row r="23" spans="1:30">
       <c r="A23" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B23" s="1"/>
       <c r="D23" s="9" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F23" s="1"/>
       <c r="I23" s="1"/>
@@ -3571,11 +3579,11 @@
     </row>
     <row r="24" spans="1:30">
       <c r="A24" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B24" s="1"/>
       <c r="D24" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -3605,11 +3613,11 @@
     </row>
     <row r="25" spans="1:30">
       <c r="A25" s="4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B25" s="1"/>
       <c r="D25" s="9" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -3639,11 +3647,11 @@
     </row>
     <row r="26" spans="1:30">
       <c r="A26" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B26" s="1"/>
       <c r="D26" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -3673,14 +3681,14 @@
     </row>
     <row r="27" spans="1:30">
       <c r="A27" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -3710,11 +3718,11 @@
     </row>
     <row r="28" spans="1:30">
       <c r="A28" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B28" s="1"/>
       <c r="D28" s="9" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -3744,11 +3752,11 @@
     </row>
     <row r="29" spans="1:30">
       <c r="A29" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B29" s="1"/>
       <c r="D29" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -3778,11 +3786,11 @@
     </row>
     <row r="30" spans="1:30">
       <c r="A30" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B30" s="1"/>
       <c r="D30" s="9" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -3812,11 +3820,11 @@
     </row>
     <row r="31" spans="1:30">
       <c r="A31" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B31" s="1"/>
       <c r="D31" s="9" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -3846,12 +3854,12 @@
     </row>
     <row r="32" spans="1:30">
       <c r="A32" s="4" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="7"/>
       <c r="D32" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -3881,12 +3889,12 @@
     </row>
     <row r="33" spans="1:30">
       <c r="A33" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="7"/>
       <c r="D33" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -3916,7 +3924,7 @@
     </row>
     <row r="34" spans="1:30">
       <c r="A34" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="7"/>
@@ -3950,7 +3958,7 @@
     </row>
     <row r="35" spans="1:30">
       <c r="A35" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="7"/>
@@ -3984,7 +3992,7 @@
     </row>
     <row r="36" spans="1:30">
       <c r="A36" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="7"/>
@@ -4018,7 +4026,7 @@
     </row>
     <row r="37" spans="1:30">
       <c r="A37" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="7"/>
@@ -4052,7 +4060,7 @@
     </row>
     <row r="38" spans="1:30">
       <c r="A38" s="4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="7"/>
@@ -4086,7 +4094,7 @@
     </row>
     <row r="39" spans="1:30">
       <c r="A39" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="7"/>
@@ -4120,7 +4128,7 @@
     </row>
     <row r="40" spans="1:30">
       <c r="A40" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="7"/>
@@ -4154,7 +4162,7 @@
     </row>
     <row r="41" spans="1:30">
       <c r="A41" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="7"/>
@@ -4188,7 +4196,7 @@
     </row>
     <row r="42" spans="1:30">
       <c r="A42" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="7"/>
@@ -4222,7 +4230,7 @@
     </row>
     <row r="43" spans="1:30">
       <c r="A43" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="7"/>
@@ -4256,7 +4264,7 @@
     </row>
     <row r="44" spans="1:30">
       <c r="A44" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="7"/>
@@ -4290,7 +4298,7 @@
     </row>
     <row r="45" spans="1:30">
       <c r="A45" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="7"/>
@@ -4324,7 +4332,7 @@
     </row>
     <row r="46" spans="1:30">
       <c r="A46" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="7"/>
@@ -4358,7 +4366,7 @@
     </row>
     <row r="47" spans="1:30">
       <c r="A47" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="7"/>
@@ -4392,7 +4400,7 @@
     </row>
     <row r="48" spans="1:30">
       <c r="A48" s="4" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="7"/>
@@ -4426,7 +4434,7 @@
     </row>
     <row r="49" spans="1:30">
       <c r="A49" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="7"/>
@@ -4460,7 +4468,7 @@
     </row>
     <row r="50" spans="1:30">
       <c r="A50" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="7"/>
@@ -4494,7 +4502,7 @@
     </row>
     <row r="51" spans="1:30">
       <c r="A51" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="7"/>
@@ -4528,7 +4536,7 @@
     </row>
     <row r="52" spans="1:30">
       <c r="A52" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="7"/>
@@ -4562,7 +4570,7 @@
     </row>
     <row r="53" spans="1:30">
       <c r="A53" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="7"/>
@@ -4596,7 +4604,7 @@
     </row>
     <row r="54" spans="1:30">
       <c r="A54" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="7"/>
@@ -4630,7 +4638,7 @@
     </row>
     <row r="55" spans="1:30">
       <c r="A55" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="7"/>
@@ -4664,7 +4672,7 @@
     </row>
     <row r="56" spans="1:30">
       <c r="A56" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="7"/>
@@ -4698,7 +4706,7 @@
     </row>
     <row r="57" spans="1:30">
       <c r="A57" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="7"/>
@@ -4732,7 +4740,7 @@
     </row>
     <row r="58" spans="1:30">
       <c r="A58" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="7"/>
@@ -4766,7 +4774,7 @@
     </row>
     <row r="59" spans="1:30">
       <c r="A59" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="7"/>
@@ -4800,7 +4808,7 @@
     </row>
     <row r="60" spans="1:30">
       <c r="A60" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="7"/>
@@ -4834,7 +4842,7 @@
     </row>
     <row r="61" spans="1:30">
       <c r="A61" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="7"/>
@@ -4868,7 +4876,7 @@
     </row>
     <row r="62" spans="1:30">
       <c r="A62" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="7"/>
@@ -4902,7 +4910,7 @@
     </row>
     <row r="63" spans="1:30">
       <c r="A63" s="4" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="7"/>
@@ -4936,7 +4944,7 @@
     </row>
     <row r="64" spans="1:30">
       <c r="A64" s="4" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="7"/>
@@ -4970,7 +4978,7 @@
     </row>
     <row r="65" spans="1:30">
       <c r="A65" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="7"/>
@@ -5004,7 +5012,7 @@
     </row>
     <row r="66" spans="1:30">
       <c r="A66" s="4" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="7"/>
@@ -5038,7 +5046,7 @@
     </row>
     <row r="67" spans="1:30">
       <c r="A67" s="4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="7"/>
@@ -5072,7 +5080,7 @@
     </row>
     <row r="68" spans="1:30">
       <c r="A68" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="7"/>
@@ -5106,7 +5114,7 @@
     </row>
     <row r="69" spans="1:30">
       <c r="A69" s="4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="7"/>
@@ -5140,7 +5148,7 @@
     </row>
     <row r="70" spans="1:30">
       <c r="A70" s="4" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="7"/>
@@ -5174,7 +5182,7 @@
     </row>
     <row r="71" spans="1:30">
       <c r="A71" s="4" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="7"/>
@@ -5208,7 +5216,7 @@
     </row>
     <row r="72" spans="1:30">
       <c r="A72" s="4" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="7"/>
@@ -5242,7 +5250,7 @@
     </row>
     <row r="73" spans="1:30">
       <c r="A73" s="4" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="7"/>
@@ -5276,7 +5284,7 @@
     </row>
     <row r="74" spans="1:30">
       <c r="A74" s="4" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="7"/>
@@ -5310,7 +5318,7 @@
     </row>
     <row r="75" spans="1:30">
       <c r="A75" s="4" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="7"/>
@@ -5344,7 +5352,7 @@
     </row>
     <row r="76" spans="1:30">
       <c r="A76" s="4" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="7"/>
@@ -5378,7 +5386,7 @@
     </row>
     <row r="77" spans="1:30">
       <c r="A77" s="4" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="7"/>
@@ -5412,7 +5420,7 @@
     </row>
     <row r="78" spans="1:30">
       <c r="A78" s="4" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="7"/>
@@ -5446,7 +5454,7 @@
     </row>
     <row r="79" spans="1:30">
       <c r="A79" s="4" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="7"/>
@@ -5480,7 +5488,7 @@
     </row>
     <row r="80" spans="1:30">
       <c r="A80" s="4" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="7"/>

</xml_diff>